<commit_message>
Added script used to generate plots and raw autocorrelation data
</commit_message>
<xml_diff>
--- a/DLSdata/20170707_MI_INP_DLS_1s_10aq_exp_t1h_t2h_all_individual_acquisitions.xlsx
+++ b/DLSdata/20170707_MI_INP_DLS_1s_10aq_exp_t1h_t2h_all_individual_acquisitions.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1020" windowWidth="25485" windowHeight="11685"/>
+    <workbookView xWindow="0" yWindow="1275" windowWidth="25485" windowHeight="11685" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="t1h" sheetId="1" r:id="rId1"/>
@@ -719,11 +719,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W1149"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1124" workbookViewId="0">
+    <sheetView topLeftCell="A972" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="K1149" sqref="K1149"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="8" max="8" width="19.140625" customWidth="1"/>
+    <col min="11" max="11" width="11.7109375" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -45297,8 +45301,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W1132"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L8" sqref="L8"/>
+    <sheetView tabSelected="1" topLeftCell="A240" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
+      <selection activeCell="E286" sqref="E286"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>